<commit_message>
change name of columns
</commit_message>
<xml_diff>
--- a/lab4-linear_regression/data.xlsx
+++ b/lab4-linear_regression/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\AppData\Local\Temp\Rar$DIa6684.25842\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R1505-We2-3-Stud\Documents\mathematical_statistic\lab4-linear_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B163AF-350F-41F9-A68A-AFAA468EE10C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{794E677D-4C19-4466-BE84-53EDDA6FB806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Height(Inches)</t>
+    <t>Height</t>
   </si>
   <si>
-    <t>Weight(Pounds)</t>
+    <t>Weight</t>
   </si>
 </sst>
 </file>
@@ -433,15 +433,15 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.36328125" style="2" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>65.78331</v>
       </c>
@@ -457,7 +457,7 @@
         <v>112.99250000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>71.515209999999996</v>
       </c>
@@ -465,7 +465,7 @@
         <v>136.4873</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>69.398740000000004</v>
       </c>
@@ -473,7 +473,7 @@
         <v>153.02690000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>68.2166</v>
       </c>
@@ -481,7 +481,7 @@
         <v>142.33539999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>67.787809999999993</v>
       </c>
@@ -489,7 +489,7 @@
         <v>144.2971</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>68.697839999999999</v>
       </c>
@@ -497,7 +497,7 @@
         <v>123.30240000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>69.802040000000005</v>
       </c>
@@ -505,7 +505,7 @@
         <v>141.49469999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>70.014719999999997</v>
       </c>
@@ -513,7 +513,7 @@
         <v>136.4623</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>67.902649999999994</v>
       </c>
@@ -521,7 +521,7 @@
         <v>112.3723</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>66.782359999999997</v>
       </c>
@@ -529,7 +529,7 @@
         <v>120.66719999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>66.487690000000001</v>
       </c>
@@ -537,7 +537,7 @@
         <v>127.4516</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>67.623329999999996</v>
       </c>
@@ -545,7 +545,7 @@
         <v>114.143</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>68.302480000000003</v>
       </c>
@@ -553,7 +553,7 @@
         <v>125.61069999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>67.116560000000007</v>
       </c>
@@ -561,7 +561,7 @@
         <v>122.4618</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>68.279669999999996</v>
       </c>
@@ -569,7 +569,7 @@
         <v>116.0866</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>71.0916</v>
       </c>
@@ -577,7 +577,7 @@
         <v>139.9975</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>66.460999999999999</v>
       </c>
@@ -585,7 +585,7 @@
         <v>129.50229999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>68.649270000000001</v>
       </c>
@@ -593,7 +593,7 @@
         <v>142.97329999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>71.230329999999995</v>
       </c>
@@ -601,7 +601,7 @@
         <v>137.9025</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>67.131180000000001</v>
       </c>
@@ -609,7 +609,7 @@
         <v>124.0449</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>67.833789999999993</v>
       </c>
@@ -617,7 +617,7 @@
         <v>141.2807</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>68.878810000000001</v>
       </c>
@@ -625,7 +625,7 @@
         <v>143.53919999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>63.48115</v>
       </c>
@@ -633,7 +633,7 @@
         <v>97.901910000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>68.421869999999998</v>
       </c>
@@ -641,7 +641,7 @@
         <v>129.5027</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>67.628039999999999</v>
       </c>
@@ -649,7 +649,7 @@
         <v>141.8501</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>67.208640000000003</v>
       </c>
@@ -657,7 +657,7 @@
         <v>129.7244</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>70.842349999999996</v>
       </c>
@@ -665,7 +665,7 @@
         <v>142.42349999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>67.494339999999994</v>
       </c>
@@ -673,7 +673,7 @@
         <v>131.55019999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>66.534009999999995</v>
       </c>
@@ -681,7 +681,7 @@
         <v>108.33240000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>65.440979999999996</v>
       </c>
@@ -689,7 +689,7 @@
         <v>113.8922</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>69.523300000000006</v>
       </c>
@@ -697,7 +697,7 @@
         <v>103.30159999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>65.813199999999995</v>
       </c>
@@ -705,7 +705,7 @@
         <v>120.75360000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>67.816299999999998</v>
       </c>
@@ -713,7 +713,7 @@
         <v>125.7886</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>70.595050000000001</v>
       </c>
@@ -721,7 +721,7 @@
         <v>136.2225</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>71.804839999999999</v>
       </c>
@@ -729,7 +729,7 @@
         <v>140.10149999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>69.206130000000002</v>
       </c>
@@ -737,7 +737,7 @@
         <v>128.74870000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>66.80368</v>
       </c>
@@ -745,7 +745,7 @@
         <v>141.79939999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>67.658929999999998</v>
       </c>
@@ -753,7 +753,7 @@
         <v>121.2319</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>67.807010000000005</v>
       </c>
@@ -761,7 +761,7 @@
         <v>131.34780000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>64.045349999999999</v>
       </c>
@@ -769,7 +769,7 @@
         <v>106.7115</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>68.574629999999999</v>
       </c>
@@ -777,7 +777,7 @@
         <v>124.35980000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>65.183570000000003</v>
       </c>
@@ -785,7 +785,7 @@
         <v>124.8591</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>69.658140000000003</v>
       </c>
@@ -793,7 +793,7 @@
         <v>139.6711</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>67.967309999999998</v>
       </c>
@@ -801,7 +801,7 @@
         <v>137.36959999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>65.980879999999999</v>
       </c>
@@ -809,7 +809,7 @@
         <v>106.4499</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>68.672489999999996</v>
       </c>
@@ -817,7 +817,7 @@
         <v>128.76390000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>66.880880000000005</v>
       </c>
@@ -825,7 +825,7 @@
         <v>145.68369999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>67.698679999999996</v>
       </c>
@@ -833,7 +833,7 @@
         <v>116.819</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>69.821169999999995</v>
       </c>
@@ -841,7 +841,7 @@
         <v>143.6215</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>69.088170000000005</v>
       </c>
@@ -849,7 +849,7 @@
         <v>134.9325</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>69.914789999999996</v>
       </c>
@@ -857,7 +857,7 @@
         <v>147.02189999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>67.331819999999993</v>
       </c>
@@ -865,7 +865,7 @@
         <v>126.32850000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>70.269390000000001</v>
       </c>
@@ -873,7 +873,7 @@
         <v>125.48390000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>69.103440000000006</v>
       </c>
@@ -881,7 +881,7 @@
         <v>115.7084</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>65.383560000000003</v>
       </c>
@@ -889,7 +889,7 @@
         <v>123.4892</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>70.184470000000005</v>
       </c>
@@ -897,7 +897,7 @@
         <v>147.89259999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>70.406170000000003</v>
       </c>
@@ -905,7 +905,7 @@
         <v>155.89869999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>66.543760000000006</v>
       </c>
@@ -913,7 +913,7 @@
         <v>128.07419999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>66.364180000000005</v>
       </c>
@@ -921,7 +921,7 @@
         <v>119.37009999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>67.537000000000006</v>
       </c>
@@ -929,7 +929,7 @@
         <v>133.81479999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>66.504180000000005</v>
       </c>
@@ -937,7 +937,7 @@
         <v>128.73249999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>68.999579999999995</v>
       </c>
@@ -945,7 +945,7 @@
         <v>137.5453</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>68.303550000000001</v>
       </c>
@@ -953,7 +953,7 @@
         <v>129.7604</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>67.012550000000005</v>
       </c>
@@ -961,7 +961,7 @@
         <v>128.82400000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>70.80592</v>
       </c>
@@ -969,7 +969,7 @@
         <v>135.31649999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>68.21951</v>
       </c>
@@ -977,7 +977,7 @@
         <v>109.6113</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>69.059139999999999</v>
       </c>
@@ -985,7 +985,7 @@
         <v>142.4684</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>67.731030000000004</v>
       </c>
@@ -993,7 +993,7 @@
         <v>132.749</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>67.215680000000006</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>103.5275</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>67.367630000000005</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>124.7299</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>65.270330000000001</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>129.31370000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>70.842780000000005</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>134.01750000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>69.924419999999998</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>140.39689999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>64.285079999999994</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>102.8351</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>68.245199999999997</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>128.5214</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>66.357079999999996</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>120.2991</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>68.362750000000005</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>138.6036</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>65.476900000000001</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>132.95740000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>69.719470000000001</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>115.6233</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>67.725539999999995</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>122.524</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>68.639409999999998</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>134.62540000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>66.784049999999993</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>121.8986</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>70.051469999999995</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>155.3767</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>66.278480000000002</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>128.9418</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>69.201980000000006</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>129.10130000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>69.134810000000002</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>139.47329999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>67.364360000000005</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>140.89009999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>70.092969999999994</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>131.5916</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>70.176599999999993</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>121.1232</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>68.225560000000002</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>131.5127</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>68.129320000000007</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>136.5479</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>70.242559999999997</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>141.4896</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>71.487520000000004</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>140.6104</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>69.204769999999996</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>112.1413</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>70.063059999999993</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>133.45699999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>70.557029999999997</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>131.80009999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>66.286439999999999</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>120.02849999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>63.42577</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>123.0972</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>66.767110000000002</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>128.14320000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>68.887410000000003</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>115.4759</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>64.874340000000004</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>102.09269999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>67.09272</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>130.35300000000001</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>68.347610000000003</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>134.1842</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>65.610730000000004</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>98.641329999999996</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>67.755510000000001</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>114.5599</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>68.021199999999993</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>123.49169999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>67.661929999999998</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>123.048</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>66.314599999999999</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>126.4772</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>69.437060000000002</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>128.417</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>63.836239999999997</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>127.19410000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>67.722769999999997</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>122.0562</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>70.050979999999996</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>127.60639999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>70.186019999999999</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>131.64230000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>65.945880000000002</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>111.8955</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>70.007000000000005</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>122.039</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>68.611289999999997</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>128.5547</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>68.808170000000004</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>132.67920000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>69.762119999999996</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>136.06319999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>65.455389999999994</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>115.94029999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>68.825339999999997</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>136.9041</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>65.800299999999993</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>119.88039999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>67.214740000000006</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>109.0055</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>69.420209999999997</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>128.2705</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>68.943960000000004</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>135.29130000000001</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>67.941500000000005</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>106.8558</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>65.625060000000005</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>123.29389999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>66.496070000000003</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>109.51430000000001</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>67.928089999999997</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>119.3087</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>68.894149999999996</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>140.24019999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>70.241</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>133.98410000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>68.266229999999993</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>132.58070000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>71.231610000000003</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>130.69880000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>69.097470000000001</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>115.5637</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>64.396929999999998</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>123.7941</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>71.095849999999999</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>128.14269999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>68.218680000000006</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>135.96459999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>65.917209999999997</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>116.62730000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>67.436899999999994</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>126.8241</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>73.901070000000004</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>151.3913</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>69.981489999999994</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>130.40219999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>69.518619999999999</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>136.20679999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>65.184370000000001</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>113.3989</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>68.008690000000001</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>125.3287</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>68.338399999999993</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>127.58459999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>65.184169999999995</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>107.1564</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>68.262090000000001</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>116.4588</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>68.568650000000005</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>133.84020000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>64.496750000000006</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>112.8901</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>68.710530000000006</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>130.7568</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>68.891480000000001</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>137.75710000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>69.540109999999999</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>125.4036</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>67.399640000000005</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>138.4659</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>66.475210000000004</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>120.8184</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>66.012169999999998</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>140.15389999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>72.444339999999997</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>136.7397</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>64.126419999999996</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>106.1139</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>70.981120000000004</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>158.9562</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>67.501239999999996</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>108.7868</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>72.015150000000006</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>138.7758</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>65.311430000000001</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>115.9136</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>67.075090000000003</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>146.29220000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>64.391480000000001</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>109.87649999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>69.37003</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>139.04990000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>68.37921</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>119.90009999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>65.310180000000003</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>128.30690000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>67.136899999999997</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>127.2428</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>68.394679999999994</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>115.2306</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>66.291799999999995</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>124.7975</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>67.186599999999999</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>126.9511</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>65.991560000000007</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>111.2711</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>69.433930000000004</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>122.60890000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>67.974630000000005</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>124.2084</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>67.761330000000001</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>124.64530000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>65.278639999999996</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>119.51690000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>73.833640000000003</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>139.29830000000001</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>66.813119999999998</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>104.8265</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>66.894109999999998</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>123.0424</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>65.735680000000002</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>118.89230000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>65.982830000000007</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>121.4939</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>66.583960000000005</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>119.2488</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>67.112939999999995</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>135.0239</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>65.874809999999997</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>116.22799999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>66.780670000000001</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>109.17310000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>68.735770000000002</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>124.22369999999999</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>66.226659999999995</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>141.1645</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>65.959680000000006</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>129.15010000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>68.58372</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>127.8693</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>66.593469999999996</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>120.92440000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>66.965739999999997</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>127.64660000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>68.080150000000003</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>101.4693</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>70.190250000000006</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>144.99270000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>65.52149</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>110.95229999999999</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>67.459050000000005</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>132.86250000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>67.409850000000006</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>146.33850000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>69.661580000000001</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>145.58940000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>65.797989999999999</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>120.84310000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>66.105580000000003</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>115.7813</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>68.239869999999996</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>128.30189999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>68.024029999999996</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>127.4718</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>71.390439999999998</v>
       </c>

</xml_diff>